<commit_message>
Thay doi file CSDL
</commit_message>
<xml_diff>
--- a/HoaDon.xlsx
+++ b/HoaDon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Mã Hoá Đơn</t>
   </si>
@@ -51,18 +51,6 @@
   </si>
   <si>
     <t>200,000 VNĐ</t>
-  </si>
-  <si>
-    <t>07/05/2025</t>
-  </si>
-  <si>
-    <t>630,000 VNĐ</t>
-  </si>
-  <si>
-    <t>08/05/2025</t>
-  </si>
-  <si>
-    <t>165,000 VNĐ</t>
   </si>
 </sst>
 </file>
@@ -107,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -196,126 +184,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C6" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="B7" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="D7" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="B8" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C8" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="D8" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n" s="0">
-        <v>8.0</v>
-      </c>
-      <c r="B9" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C9" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n" s="0">
-        <v>9.0</v>
-      </c>
-      <c r="B10" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C10" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="D10" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>